<commit_message>
fixed underscore of spreadsheet
</commit_message>
<xml_diff>
--- a/Toy_Dataset_Input_and_Output.xlsx
+++ b/Toy_Dataset_Input_and_Output.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justin/Google Drive/4th Year/Ciernia Lab/Shiny_Applications/FinalUploadedApp/MGEnrichmentApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23CAEEE-ABD4-554C-ACBA-C977DE691462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94623B5-DB88-2E4E-9901-87A638BE84C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ASD&gt;CTRL_DEGs _Dataset" sheetId="4" r:id="rId1"/>
-    <sheet name="ASD&gt;CTRL_DEGs _Results" sheetId="8" r:id="rId2"/>
-    <sheet name="ASD&lt;CTRL_DEGs _Dataset" sheetId="5" r:id="rId3"/>
-    <sheet name="ASD&lt;CTRL_DEGs _Results" sheetId="7" r:id="rId4"/>
+    <sheet name="ASD&gt;CTRL_DEGs_Dataset" sheetId="4" r:id="rId1"/>
+    <sheet name="ASD&gt;CTRL_DEGs_Results" sheetId="8" r:id="rId2"/>
+    <sheet name="ASD&lt;CTRL_DEGs_Dataset" sheetId="5" r:id="rId3"/>
+    <sheet name="ASD&lt;CTRL_DEGs_Results" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -3279,7 +3279,7 @@
   <dimension ref="A1:A199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4288,7 +4288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EE4E8E-7C26-3249-93A1-83BB9A9A9312}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -6956,7 +6956,7 @@
   <dimension ref="A1:A181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7875,8 +7875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553C8F2E-F545-D24C-B9AA-B9E4A60FD210}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>